<commit_message>
Slides for week 7
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -492,7 +492,26 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve">)
+- [ ] (Optional) [Manufacturer’s Guide to Developing Consumer Product Instructions](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">https://www.cpsc.gov/s3fs-public/pdfs/guide.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) - Excellent guide to writing user guides
+</t>
     </r>
   </si>
   <si>
@@ -502,11 +521,11 @@
     <t xml:space="preserve">- [ ] For Wednesday: Submit a needs assessment and task analysis for your user guide.</t>
   </si>
   <si>
-    <t xml:space="preserve">- Describing statistical methods
-- Writing good “how to” guides for others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Documenting code </t>
+    <t xml:space="preserve">- [Describing statistical methods](../slides/07-statistical-methods.qmd)
+- Documenting code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Writing good “how to” guides for others</t>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Work on your user guide (due next week!)</t>
@@ -1257,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1469,7 +1488,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="216.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="271.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -1491,7 +1510,7 @@
       <c r="G8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="6" t="s">
         <v>54</v>
       </c>
       <c r="I8" s="1" t="s">

</xml_diff>

<commit_message>
graphs/charts and diagrams slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -525,7 +525,7 @@
 - Documenting code</t>
   </si>
   <si>
-    <t xml:space="preserve">- Writing good “how to” guides for others</t>
+    <t xml:space="preserve">- [Writing good “how to” guides for others](../slides/07-user-guides.qmd)</t>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Work on your user guide (due next week!)</t>
@@ -600,11 +600,11 @@
     <t xml:space="preserve">- [ ] Reading Quiz Week 8</t>
   </si>
   <si>
-    <t xml:space="preserve">- Tables and charts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Diagrams
-- IKEA-style assembly diagram assessment</t>
+    <t xml:space="preserve">- [Tables and charts](../slides/08-tables-charts.qmd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Diagrams](.../slides/08-diagrams.qmd)
+- Peer review time – User guide</t>
   </si>
   <si>
     <t xml:space="preserve">- (not turned in) Work on analysis and relevant graphics for your business report</t>
@@ -1276,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updates to website -- online classes due to weather
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -342,7 +342,8 @@
     - Basic components of argument and rhetoric in scientific writing</t>
   </si>
   <si>
-    <t xml:space="preserve">- In class activity: Arguments in scientific and technical writing</t>
+    <t xml:space="preserve">- In class activity: [Arguments in scientific and technical writing](../activities/arguments.qmd)
+  - [Slides](../slides/05-argument-activity.qmd)</t>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Analyze the rhetorical decisions and arguments in your research article (1 pg summary)
@@ -1336,8 +1337,8 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updates -- week 9 slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="137">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -663,11 +663,40 @@
     <t xml:space="preserve">- [ ] Reading Quiz Week 9</t>
   </si>
   <si>
-    <t xml:space="preserve">- Describing results -- level of detail and role of supplementary documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Integrating results and visual aids
-- Countering misunderstandings</t>
+    <t xml:space="preserve">- [ ] For Wednesday: On Canvas, find the [**Activity: IgNobel Results Sections** page](https://canvas.unl.edu/courses/192983/pages). Download your assigned paper and skim through it to prepare for class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Countering misconceptions in results](../slides/09-misconceptions.qmd)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [IgNobel Results Section Activity](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://canvas.unl.edu/courses/192983/pages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) activity (Canvas) and class discussion</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Draft of results section of business report with relevant graphics/visual aids</t>
@@ -1337,8 +1366,8 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1604,7 +1633,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="68.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -1620,14 +1649,17 @@
       <c r="E10" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="92.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,22 +1670,22 @@
         <v>45747</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,25 +1696,25 @@
         <v>45754</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,22 +1725,22 @@
         <v>45761</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,22 +1751,22 @@
         <v>45768</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="171.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,25 +1777,25 @@
         <v>45775</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="59.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,16 +1806,16 @@
         <v>45782</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1793,6 +1825,7 @@
     <hyperlink ref="H3" r:id="rId3" display="- Peer Review CV/cover letter&#10;- Discuss how to give good feedback (based on [ETC](https://wisc.pb.unizin.org/opencomp/chapter/providing-good-feedback/))"/>
     <hyperlink ref="D4" r:id="rId4" display="- [ ] Read [OTC Chapter 5.6 – References](https://alg.manifoldapp.org/read/open-technical-communication/section/d9202f07-41a2-4dc9-8b29-486e164c1775)  &#10;- [ ] Read [OTC Chapter 3 - Ethics](https://alg.manifoldapp.org/read/open-technical-communication/section/8b530f4b-5942-4071-845a-0a138601da10)  &#10;- [ ] Read [ETC Annoying Ways People Use Sources](https://wisc.pb.unizin.org/opencomp/chapter/annoying-ways-people-use-sources/)&#10;- [ ] Practical Tutorial: [Connecting Rstudio + Zotero](https://gsverhoeven.github.io/post/zotero-rmarkdown-csl/)"/>
     <hyperlink ref="D10" r:id="rId5" display="- [ ] Read [SWHR 5 - Results](https://ehsanx.github.io/Scientific-Writing-for-Health-Research/results-section.html)"/>
+    <hyperlink ref="H10" r:id="rId6" display="https://canvas.unl.edu/courses/192983/pages"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1811,7 +1844,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1819,16 +1852,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,13 +1869,13 @@
         <v>20250314</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,13 +1883,13 @@
         <v>20250425</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,13 +1897,13 @@
         <v>20250504</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1879,13 +1912,13 @@
         <v>20250310</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1894,13 +1927,13 @@
         <v>20250505</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1922,7 +1955,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1933,21 +1966,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>20250120</v>
@@ -1958,7 +1991,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20250120</v>
@@ -1966,7 +1999,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20250316</v>
@@ -1977,7 +2010,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20250512</v>
@@ -1988,10 +2021,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2012,7 +2045,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2020,68 +2053,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates - week 11 slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -800,10 +800,11 @@
     <t xml:space="preserve">- [ ] For Wednesday: Find 2 articles about how to write an executive summary, one from an educational resource (a university) and one from a business or professional resource (e.g. LinkedIn, Adobe, etc.). What do they have in common? What recommendations conflict?</t>
   </si>
   <si>
-    <t xml:space="preserve">- Abstracts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Executive Summaries - Class discussion</t>
+    <t xml:space="preserve">- [Abstracts](../slides/11-abstract.qmd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Executive Summaries](../slides/11-exec-summary.qmd)
+- Class Discussion</t>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Draft of executive summary of business report</t>

</xml_diff>

<commit_message>
Update website -- week 12 slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="136">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -886,10 +886,7 @@
     <t xml:space="preserve">- [ ] Reading Quiz Week 12</t>
   </si>
   <si>
-    <t xml:space="preserve">- Logical fallacies in the workplace in-class activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Statistical misunderstandings and how to counter them -- class discussion</t>
+    <t xml:space="preserve">- [Case Study - Statistical Ethics](../slides/12-ethics.qmd)</t>
   </si>
   <si>
     <t xml:space="preserve">- (not turned in) Revise business report sections (methods, results, intro, conclusion, executive summary) and prepare to integrate them into a full report</t>
@@ -1341,8 +1338,8 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1692,7 +1689,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -1712,10 +1709,10 @@
         <v>85</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="104" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,22 +1723,22 @@
         <v>45768</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="171.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,25 +1749,25 @@
         <v>45775</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="59.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1781,16 +1778,16 @@
         <v>45782</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1819,7 +1816,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1827,16 +1824,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,13 +1841,13 @@
         <v>20250314</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,13 +1855,13 @@
         <v>20250425</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,13 +1869,13 @@
         <v>20250504</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -1887,13 +1884,13 @@
         <v>20250310</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -1902,13 +1899,13 @@
         <v>20250505</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -1930,7 +1927,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1941,21 +1938,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>20250120</v>
@@ -1966,7 +1963,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20250120</v>
@@ -1974,7 +1971,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20250316</v>
@@ -1985,7 +1982,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20250512</v>
@@ -1996,10 +1993,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2020,7 +2017,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2028,68 +2025,68 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>